<commit_message>
hacked a corner LUT
multiplied top row and left side LUTs to get top left corner LUT (and
then mirrored that around and filled in the 4D LUT)
</commit_message>
<xml_diff>
--- a/IC_Solar/Shading_LUT/Generic_8x8/pctExposedLUT_module_08.xlsx
+++ b/IC_Solar/Shading_LUT/Generic_8x8/pctExposedLUT_module_08.xlsx
@@ -33,8 +33,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -62,8 +70,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -347,10 +356,13 @@
   <dimension ref="A1:AX50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="Y48" sqref="Y48"/>
+      <selection activeCell="Y30" sqref="Y30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="25" max="25" width="8.88671875" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:50" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -425,7 +437,7 @@
       <c r="X1">
         <v>-6</v>
       </c>
-      <c r="Y1">
+      <c r="Y1" s="1">
         <v>-3</v>
       </c>
       <c r="Z1">
@@ -577,7 +589,7 @@
       <c r="X2">
         <v>2.5862000000000052E-2</v>
       </c>
-      <c r="Y2">
+      <c r="Y2" s="1">
         <v>2.5862000000000052E-2</v>
       </c>
       <c r="Z2">
@@ -729,7 +741,7 @@
       <c r="X3">
         <v>7.7586000000000044E-2</v>
       </c>
-      <c r="Y3">
+      <c r="Y3" s="1">
         <v>7.7586000000000044E-2</v>
       </c>
       <c r="Z3">
@@ -881,7 +893,7 @@
       <c r="X4">
         <v>0.13793100000000003</v>
       </c>
-      <c r="Y4">
+      <c r="Y4" s="1">
         <v>0.13793100000000003</v>
       </c>
       <c r="Z4">
@@ -1033,7 +1045,7 @@
       <c r="X5">
         <v>0.18103400000000003</v>
       </c>
-      <c r="Y5">
+      <c r="Y5" s="1">
         <v>0.18965500000000002</v>
       </c>
       <c r="Z5">
@@ -1185,7 +1197,7 @@
       <c r="X6">
         <v>0.23275900000000005</v>
       </c>
-      <c r="Y6">
+      <c r="Y6" s="1">
         <v>0.24137900000000001</v>
       </c>
       <c r="Z6">
@@ -1337,7 +1349,7 @@
       <c r="X7">
         <v>0.293103</v>
       </c>
-      <c r="Y7">
+      <c r="Y7" s="1">
         <v>0.30172399999999999</v>
       </c>
       <c r="Z7">
@@ -1489,7 +1501,7 @@
       <c r="X8">
         <v>0.35344799999999998</v>
       </c>
-      <c r="Y8">
+      <c r="Y8" s="1">
         <v>0.35344799999999998</v>
       </c>
       <c r="Z8">
@@ -1641,7 +1653,7 @@
       <c r="X9">
         <v>0.40517199999999998</v>
       </c>
-      <c r="Y9">
+      <c r="Y9" s="1">
         <v>0.40517199999999998</v>
       </c>
       <c r="Z9">
@@ -1793,7 +1805,7 @@
       <c r="X10">
         <v>0.456897</v>
       </c>
-      <c r="Y10">
+      <c r="Y10" s="1">
         <v>0.456897</v>
       </c>
       <c r="Z10">
@@ -1945,7 +1957,7 @@
       <c r="X11">
         <v>0.52586200000000005</v>
       </c>
-      <c r="Y11">
+      <c r="Y11" s="1">
         <v>0.52586200000000005</v>
       </c>
       <c r="Z11">
@@ -2097,7 +2109,7 @@
       <c r="X12">
         <v>0.56896600000000008</v>
       </c>
-      <c r="Y12">
+      <c r="Y12" s="1">
         <v>0.57758599999999993</v>
       </c>
       <c r="Z12">
@@ -2249,7 +2261,7 @@
       <c r="X13">
         <v>0.62931000000000004</v>
       </c>
-      <c r="Y13">
+      <c r="Y13" s="1">
         <v>0.62068999999999996</v>
       </c>
       <c r="Z13">
@@ -2401,7 +2413,7 @@
       <c r="X14">
         <v>0.68103399999999992</v>
       </c>
-      <c r="Y14">
+      <c r="Y14" s="1">
         <v>0.68103399999999992</v>
       </c>
       <c r="Z14">
@@ -2553,7 +2565,7 @@
       <c r="X15">
         <v>0.74137900000000001</v>
       </c>
-      <c r="Y15">
+      <c r="Y15" s="1">
         <v>0.75</v>
       </c>
       <c r="Z15">
@@ -2705,7 +2717,7 @@
       <c r="X16">
         <v>0.793103</v>
       </c>
-      <c r="Y16">
+      <c r="Y16" s="1">
         <v>0.793103</v>
       </c>
       <c r="Z16">
@@ -2857,7 +2869,7 @@
       <c r="X17">
         <v>0.84482800000000002</v>
       </c>
-      <c r="Y17">
+      <c r="Y17" s="1">
         <v>0.84482800000000002</v>
       </c>
       <c r="Z17">
@@ -3009,7 +3021,7 @@
       <c r="X18">
         <v>0.89655200000000002</v>
       </c>
-      <c r="Y18">
+      <c r="Y18" s="1">
         <v>0.91379299999999997</v>
       </c>
       <c r="Z18">
@@ -3161,7 +3173,7 @@
       <c r="X19">
         <v>0.956897</v>
       </c>
-      <c r="Y19">
+      <c r="Y19" s="1">
         <v>0.956897</v>
       </c>
       <c r="Z19">
@@ -3313,7 +3325,7 @@
       <c r="X20">
         <v>1</v>
       </c>
-      <c r="Y20">
+      <c r="Y20" s="1">
         <v>1</v>
       </c>
       <c r="Z20">
@@ -3465,7 +3477,7 @@
       <c r="X21">
         <v>1</v>
       </c>
-      <c r="Y21">
+      <c r="Y21" s="1">
         <v>1</v>
       </c>
       <c r="Z21">
@@ -3617,7 +3629,7 @@
       <c r="X22">
         <v>1</v>
       </c>
-      <c r="Y22">
+      <c r="Y22" s="1">
         <v>1</v>
       </c>
       <c r="Z22">
@@ -3769,7 +3781,7 @@
       <c r="X23">
         <v>1</v>
       </c>
-      <c r="Y23">
+      <c r="Y23" s="1">
         <v>1</v>
       </c>
       <c r="Z23">
@@ -3921,7 +3933,7 @@
       <c r="X24">
         <v>1</v>
       </c>
-      <c r="Y24">
+      <c r="Y24" s="1">
         <v>1</v>
       </c>
       <c r="Z24">
@@ -4073,7 +4085,7 @@
       <c r="X25">
         <v>1</v>
       </c>
-      <c r="Y25">
+      <c r="Y25" s="1">
         <v>1</v>
       </c>
       <c r="Z25">
@@ -4152,155 +4164,155 @@
         <v>0.42241399999999996</v>
       </c>
     </row>
-    <row r="26" spans="1:50" x14ac:dyDescent="0.3">
-      <c r="A26">
+    <row r="26" spans="1:50" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
         <v>0</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <v>0.293103</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
         <v>0.41379299999999997</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="1">
         <v>0.46551699999999996</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="1">
         <v>0.543103</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="1">
         <v>0.58620699999999992</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="1">
         <v>0.62068999999999996</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="1">
         <v>0.69827600000000001</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="1">
         <v>0.75</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="1">
         <v>0.793103</v>
       </c>
-      <c r="K26">
+      <c r="K26" s="1">
         <v>0.82758599999999993</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="1">
         <v>0.87068999999999996</v>
       </c>
-      <c r="M26">
+      <c r="M26" s="1">
         <v>0.91379299999999997</v>
       </c>
-      <c r="N26">
+      <c r="N26" s="1">
         <v>0.956897</v>
       </c>
-      <c r="O26">
-        <v>1</v>
-      </c>
-      <c r="P26">
-        <v>1</v>
-      </c>
-      <c r="Q26">
-        <v>1</v>
-      </c>
-      <c r="R26">
-        <v>1</v>
-      </c>
-      <c r="S26">
-        <v>1</v>
-      </c>
-      <c r="T26">
-        <v>1</v>
-      </c>
-      <c r="U26">
-        <v>1</v>
-      </c>
-      <c r="V26">
-        <v>1</v>
-      </c>
-      <c r="W26">
-        <v>1</v>
-      </c>
-      <c r="X26">
-        <v>1</v>
-      </c>
-      <c r="Y26">
-        <v>1</v>
-      </c>
-      <c r="Z26">
-        <v>1</v>
-      </c>
-      <c r="AA26">
-        <v>1</v>
-      </c>
-      <c r="AB26">
-        <v>1</v>
-      </c>
-      <c r="AC26">
-        <v>1</v>
-      </c>
-      <c r="AD26">
-        <v>1</v>
-      </c>
-      <c r="AE26">
-        <v>1</v>
-      </c>
-      <c r="AF26">
-        <v>1</v>
-      </c>
-      <c r="AG26">
-        <v>1</v>
-      </c>
-      <c r="AH26">
-        <v>1</v>
-      </c>
-      <c r="AI26">
-        <v>1</v>
-      </c>
-      <c r="AJ26">
-        <v>1</v>
-      </c>
-      <c r="AK26">
-        <v>1</v>
-      </c>
-      <c r="AL26">
+      <c r="O26" s="1">
+        <v>1</v>
+      </c>
+      <c r="P26" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="1">
+        <v>1</v>
+      </c>
+      <c r="R26" s="1">
+        <v>1</v>
+      </c>
+      <c r="S26" s="1">
+        <v>1</v>
+      </c>
+      <c r="T26" s="1">
+        <v>1</v>
+      </c>
+      <c r="U26" s="1">
+        <v>1</v>
+      </c>
+      <c r="V26" s="1">
+        <v>1</v>
+      </c>
+      <c r="W26" s="1">
+        <v>1</v>
+      </c>
+      <c r="X26" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y26" s="1">
+        <v>1</v>
+      </c>
+      <c r="Z26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AA26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AB26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AC26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AD26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AE26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AG26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AK26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AL26" s="1">
         <v>0.956897</v>
       </c>
-      <c r="AM26">
+      <c r="AM26" s="1">
         <v>0.91379299999999997</v>
       </c>
-      <c r="AN26">
+      <c r="AN26" s="1">
         <v>0.87068999999999996</v>
       </c>
-      <c r="AO26">
+      <c r="AO26" s="1">
         <v>0.82758599999999993</v>
       </c>
-      <c r="AP26">
+      <c r="AP26" s="1">
         <v>0.793103</v>
       </c>
-      <c r="AQ26">
+      <c r="AQ26" s="1">
         <v>0.75</v>
       </c>
-      <c r="AR26">
+      <c r="AR26" s="1">
         <v>0.706897</v>
       </c>
-      <c r="AS26">
+      <c r="AS26" s="1">
         <v>0.66379300000000008</v>
       </c>
-      <c r="AT26">
+      <c r="AT26" s="1">
         <v>0.59482800000000002</v>
       </c>
-      <c r="AU26">
+      <c r="AU26" s="1">
         <v>0.543103</v>
       </c>
-      <c r="AV26">
+      <c r="AV26" s="1">
         <v>0.5</v>
       </c>
-      <c r="AW26">
+      <c r="AW26" s="1">
         <v>0.42241399999999996</v>
       </c>
-      <c r="AX26">
+      <c r="AX26" s="1">
         <v>0.37931000000000004</v>
       </c>
     </row>
@@ -4377,7 +4389,7 @@
       <c r="X27">
         <v>1</v>
       </c>
-      <c r="Y27">
+      <c r="Y27" s="1">
         <v>1</v>
       </c>
       <c r="Z27">
@@ -4529,7 +4541,7 @@
       <c r="X28">
         <v>1</v>
       </c>
-      <c r="Y28">
+      <c r="Y28" s="1">
         <v>1</v>
       </c>
       <c r="Z28">
@@ -4681,7 +4693,7 @@
       <c r="X29">
         <v>1</v>
       </c>
-      <c r="Y29">
+      <c r="Y29" s="1">
         <v>1</v>
       </c>
       <c r="Z29">
@@ -4833,7 +4845,7 @@
       <c r="X30">
         <v>1</v>
       </c>
-      <c r="Y30">
+      <c r="Y30" s="1">
         <v>1</v>
       </c>
       <c r="Z30">
@@ -4985,7 +4997,7 @@
       <c r="X31">
         <v>1</v>
       </c>
-      <c r="Y31">
+      <c r="Y31" s="1">
         <v>1</v>
       </c>
       <c r="Z31">
@@ -5137,7 +5149,7 @@
       <c r="X32">
         <v>1</v>
       </c>
-      <c r="Y32">
+      <c r="Y32" s="1">
         <v>1</v>
       </c>
       <c r="Z32">
@@ -5289,7 +5301,7 @@
       <c r="X33">
         <v>1</v>
       </c>
-      <c r="Y33">
+      <c r="Y33" s="1">
         <v>1</v>
       </c>
       <c r="Z33">
@@ -5441,7 +5453,7 @@
       <c r="X34">
         <v>1</v>
       </c>
-      <c r="Y34">
+      <c r="Y34" s="1">
         <v>1</v>
       </c>
       <c r="Z34">
@@ -5593,7 +5605,7 @@
       <c r="X35">
         <v>0.96551699999999996</v>
       </c>
-      <c r="Y35">
+      <c r="Y35" s="1">
         <v>0.96551699999999996</v>
       </c>
       <c r="Z35">
@@ -5745,7 +5757,7 @@
       <c r="X36">
         <v>0.956897</v>
       </c>
-      <c r="Y36">
+      <c r="Y36" s="1">
         <v>0.956897</v>
       </c>
       <c r="Z36">
@@ -5897,7 +5909,7 @@
       <c r="X37">
         <v>0.91379299999999997</v>
       </c>
-      <c r="Y37">
+      <c r="Y37" s="1">
         <v>0.91379299999999997</v>
       </c>
       <c r="Z37">
@@ -6049,7 +6061,7 @@
       <c r="X38">
         <v>0.87068999999999996</v>
       </c>
-      <c r="Y38">
+      <c r="Y38" s="1">
         <v>0.87068999999999996</v>
       </c>
       <c r="Z38">
@@ -6201,7 +6213,7 @@
       <c r="X39">
         <v>0.83620700000000003</v>
       </c>
-      <c r="Y39">
+      <c r="Y39" s="1">
         <v>0.83620700000000003</v>
       </c>
       <c r="Z39">
@@ -6353,7 +6365,7 @@
       <c r="X40">
         <v>0.81034499999999998</v>
       </c>
-      <c r="Y40">
+      <c r="Y40" s="1">
         <v>0.81034499999999998</v>
       </c>
       <c r="Z40">
@@ -6505,7 +6517,7 @@
       <c r="X41">
         <v>0.78448300000000004</v>
       </c>
-      <c r="Y41">
+      <c r="Y41" s="1">
         <v>0.78448300000000004</v>
       </c>
       <c r="Z41">
@@ -6657,7 +6669,7 @@
       <c r="X42">
         <v>0.73275899999999994</v>
       </c>
-      <c r="Y42">
+      <c r="Y42" s="1">
         <v>0.73275899999999994</v>
       </c>
       <c r="Z42">
@@ -6809,7 +6821,7 @@
       <c r="X43">
         <v>0.68965500000000002</v>
       </c>
-      <c r="Y43">
+      <c r="Y43" s="1">
         <v>0.68965500000000002</v>
       </c>
       <c r="Z43">
@@ -6961,7 +6973,7 @@
       <c r="X44">
         <v>0.63793100000000003</v>
       </c>
-      <c r="Y44">
+      <c r="Y44" s="1">
         <v>0.63793100000000003</v>
       </c>
       <c r="Z44">
@@ -7113,7 +7125,7 @@
       <c r="X45">
         <v>0.58620699999999992</v>
       </c>
-      <c r="Y45">
+      <c r="Y45" s="1">
         <v>0.58620699999999992</v>
       </c>
       <c r="Z45">
@@ -7265,7 +7277,7 @@
       <c r="X46">
         <v>0.543103</v>
       </c>
-      <c r="Y46">
+      <c r="Y46" s="1">
         <v>0.543103</v>
       </c>
       <c r="Z46">
@@ -7417,7 +7429,7 @@
       <c r="X47">
         <v>0.5</v>
       </c>
-      <c r="Y47">
+      <c r="Y47" s="1">
         <v>0.5</v>
       </c>
       <c r="Z47">
@@ -7569,7 +7581,7 @@
       <c r="X48">
         <v>0.456897</v>
       </c>
-      <c r="Y48">
+      <c r="Y48" s="1">
         <v>0.456897</v>
       </c>
       <c r="Z48">
@@ -7721,7 +7733,7 @@
       <c r="X49">
         <v>0.38793100000000003</v>
       </c>
-      <c r="Y49">
+      <c r="Y49" s="1">
         <v>0.38793100000000003</v>
       </c>
       <c r="Z49">
@@ -7873,7 +7885,7 @@
       <c r="X50">
         <v>0.33620700000000003</v>
       </c>
-      <c r="Y50">
+      <c r="Y50" s="1">
         <v>0.33620700000000003</v>
       </c>
       <c r="Z50">

</xml_diff>